<commit_message>
New version of summary stats
</commit_message>
<xml_diff>
--- a/02_TP_Equipes/TP5_NKWA_FRANK_DIABANG_SECK/outputs/CMR_LCRPGR_regions_GADM1_2015_2020_GHSL.xlsx
+++ b/02_TP_Equipes/TP5_NKWA_FRANK_DIABANG_SECK/outputs/CMR_LCRPGR_regions_GADM1_2015_2020_GHSL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\AppData\Local\Microsoft\Windows\INetCache\IE\WBVEBP9U\TP5_NKWA_FRANK_DIABANG_SECK[1]\TP5_NKWA_FRANK_DIABANG_SECK\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ISE1 CL\Semestre1\Statistiques Exploratoires Spatiales\TP\TP_Groupe\TP5\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982A2F0F-CB0F-48C6-9D6E-7934EC6FF45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B76535-C845-4979-A5F5-8B3F9A2EACE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9F570656-ACC6-47E1-9749-DBFC1762D63A}"/>
   </bookViews>
@@ -16,16 +16,11 @@
     <sheet name="CMR_LCRPGR_regions_GADM1_2015_2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="125">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -123,217 +118,283 @@
     <t>Sud-Ouest</t>
   </si>
   <si>
-    <t>0.02989374409</t>
-  </si>
-  <si>
-    <t>1.00303941</t>
-  </si>
-  <si>
-    <t>0.02980316008</t>
-  </si>
-  <si>
-    <t>39811.34289</t>
-  </si>
-  <si>
-    <t>46208.68046</t>
-  </si>
-  <si>
-    <t>1.148656725</t>
-  </si>
-  <si>
-    <t>1.320344976</t>
-  </si>
-  <si>
-    <t>0.02166245901</t>
-  </si>
-  <si>
-    <t>0.6333123511</t>
-  </si>
-  <si>
-    <t>0.03420501586</t>
-  </si>
-  <si>
-    <t>145791.8191</t>
-  </si>
-  <si>
-    <t>172984.9829</t>
-  </si>
-  <si>
-    <t>4.459115188</t>
-  </si>
-  <si>
-    <t>4.942092188</t>
-  </si>
-  <si>
-    <t>0.05294029777</t>
-  </si>
-  <si>
-    <t>1.902065998</t>
-  </si>
-  <si>
-    <t>0.02783304987</t>
-  </si>
-  <si>
-    <t>33925.95149</t>
-  </si>
-  <si>
-    <t>38991.57127</t>
-  </si>
-  <si>
-    <t>0.9972209961</t>
-  </si>
-  <si>
-    <t>1.261186878</t>
-  </si>
-  <si>
-    <t>0.06720744726</t>
-  </si>
-  <si>
-    <t>2.172267538</t>
-  </si>
-  <si>
     <t>Extrême-Nord</t>
   </si>
   <si>
-    <t>0.03093884436</t>
-  </si>
-  <si>
-    <t>139196.6206</t>
-  </si>
-  <si>
-    <t>162484.3504</t>
-  </si>
-  <si>
-    <t>2.427165843</t>
-  </si>
-  <si>
-    <t>3.242783945</t>
-  </si>
-  <si>
-    <t>0.01497433118</t>
-  </si>
-  <si>
-    <t>0.5420295694</t>
-  </si>
-  <si>
-    <t>0.02762641012</t>
-  </si>
-  <si>
-    <t>111631.3974</t>
-  </si>
-  <si>
-    <t>128167.0383</t>
-  </si>
-  <si>
-    <t>3.697901384</t>
-  </si>
-  <si>
-    <t>3.974769384</t>
-  </si>
-  <si>
-    <t>0.05846755489</t>
-  </si>
-  <si>
-    <t>1.538343326</t>
-  </si>
-  <si>
-    <t>0.03800683106</t>
-  </si>
-  <si>
-    <t>85187.94806</t>
-  </si>
-  <si>
-    <t>103017.0104</t>
-  </si>
-  <si>
-    <t>1.565623502</t>
-  </si>
-  <si>
-    <t>2.023314392</t>
-  </si>
-  <si>
-    <t>0.0717818518</t>
-  </si>
-  <si>
-    <t>3.566731494</t>
-  </si>
-  <si>
-    <t>0.02012538704</t>
-  </si>
-  <si>
-    <t>70503.93974</t>
-  </si>
-  <si>
-    <t>77967.76924</t>
-  </si>
-  <si>
-    <t>2.741011635</t>
-  </si>
-  <si>
-    <t>3.72478609</t>
-  </si>
-  <si>
-    <t>0.02242463139</t>
-  </si>
-  <si>
-    <t>1.732206433</t>
-  </si>
-  <si>
-    <t>0.01294570379</t>
-  </si>
-  <si>
-    <t>64456.84515</t>
-  </si>
-  <si>
-    <t>68767.03251</t>
-  </si>
-  <si>
-    <t>5.673077796</t>
-  </si>
-  <si>
-    <t>6.309161188</t>
-  </si>
-  <si>
-    <t>0.01785774814</t>
-  </si>
-  <si>
-    <t>1.83274715</t>
-  </si>
-  <si>
-    <t>0.009743705308</t>
-  </si>
-  <si>
-    <t>22524.28304</t>
-  </si>
-  <si>
-    <t>23648.80299</t>
-  </si>
-  <si>
-    <t>0.583475451</t>
-  </si>
-  <si>
-    <t>0.6355732392</t>
-  </si>
-  <si>
-    <t>0.02497633943</t>
-  </si>
-  <si>
-    <t>0.863416443</t>
-  </si>
-  <si>
-    <t>0.02892733817</t>
-  </si>
-  <si>
-    <t>57577.60323</t>
-  </si>
-  <si>
-    <t>66537.8095</t>
-  </si>
-  <si>
-    <t>1.555525016</t>
-  </si>
-  <si>
-    <t>1.74978162</t>
+    <t>Area_km2</t>
+  </si>
+  <si>
+    <t>Built_pct</t>
+  </si>
+  <si>
+    <t>64256.30929</t>
+  </si>
+  <si>
+    <t>0.1010290125</t>
+  </si>
+  <si>
+    <t>0.02794052509</t>
+  </si>
+  <si>
+    <t>0.9332149611</t>
+  </si>
+  <si>
+    <t>0.0299400741</t>
+  </si>
+  <si>
+    <t>1036315.167</t>
+  </si>
+  <si>
+    <t>1203665.74</t>
+  </si>
+  <si>
+    <t>56.96004669</t>
+  </si>
+  <si>
+    <t>64.91751475</t>
+  </si>
+  <si>
+    <t>69100.76442</t>
+  </si>
+  <si>
+    <t>0.3048509485</t>
+  </si>
+  <si>
+    <t>0.01899858825</t>
+  </si>
+  <si>
+    <t>0.5562228057</t>
+  </si>
+  <si>
+    <t>0.03415643525</t>
+  </si>
+  <si>
+    <t>3606065.247</t>
+  </si>
+  <si>
+    <t>4277631.185</t>
+  </si>
+  <si>
+    <t>192.379629</t>
+  </si>
+  <si>
+    <t>210.6543358</t>
+  </si>
+  <si>
+    <t>109421.7244</t>
+  </si>
+  <si>
+    <t>0.05548668215</t>
+  </si>
+  <si>
+    <t>0.04937999771</t>
+  </si>
+  <si>
+    <t>1.768948541</t>
+  </si>
+  <si>
+    <t>0.02791488648</t>
+  </si>
+  <si>
+    <t>861084.953</t>
+  </si>
+  <si>
+    <t>990062.032</t>
+  </si>
+  <si>
+    <t>48.69234498</t>
+  </si>
+  <si>
+    <t>60.7144844</t>
+  </si>
+  <si>
+    <t>34431.03773</t>
+  </si>
+  <si>
+    <t>0.4685815053</t>
+  </si>
+  <si>
+    <t>0.04799429913</t>
+  </si>
+  <si>
+    <t>1.553631521</t>
+  </si>
+  <si>
+    <t>0.0308916873</t>
+  </si>
+  <si>
+    <t>3440301.796</t>
+  </si>
+  <si>
+    <t>4014920.858</t>
+  </si>
+  <si>
+    <t>130.1138578</t>
+  </si>
+  <si>
+    <t>161.3374749</t>
+  </si>
+  <si>
+    <t>20215.57405</t>
+  </si>
+  <si>
+    <t>0.6292511735</t>
+  </si>
+  <si>
+    <t>0.01667484598</t>
+  </si>
+  <si>
+    <t>0.6061263785</t>
+  </si>
+  <si>
+    <t>0.02751051031</t>
+  </si>
+  <si>
+    <t>2836621.767</t>
+  </si>
+  <si>
+    <t>3254915.701</t>
+  </si>
+  <si>
+    <t>117.4171707</t>
+  </si>
+  <si>
+    <t>127.2067369</t>
+  </si>
+  <si>
+    <t>66633.45304</t>
+  </si>
+  <si>
+    <t>0.1494374971</t>
+  </si>
+  <si>
+    <t>0.04474959651</t>
+  </si>
+  <si>
+    <t>1.17673299</t>
+  </si>
+  <si>
+    <t>0.03802867506</t>
+  </si>
+  <si>
+    <t>2071164.938</t>
+  </si>
+  <si>
+    <t>2504914.485</t>
+  </si>
+  <si>
+    <t>81.36917558</t>
+  </si>
+  <si>
+    <t>99.57536446</t>
+  </si>
+  <si>
+    <t>17530.73329</t>
+  </si>
+  <si>
+    <t>0.8502037489</t>
+  </si>
+  <si>
+    <t>0.0558525501</t>
+  </si>
+  <si>
+    <t>2.765397863</t>
+  </si>
+  <si>
+    <t>0.0201969311</t>
+  </si>
+  <si>
+    <t>1723681.743</t>
+  </si>
+  <si>
+    <t>1906839.591</t>
+  </si>
+  <si>
+    <t>116.510038</t>
+  </si>
+  <si>
+    <t>149.0469516</t>
+  </si>
+  <si>
+    <t>13953.00128</t>
+  </si>
+  <si>
+    <t>1.703106909</t>
+  </si>
+  <si>
+    <t>0.01423361285</t>
+  </si>
+  <si>
+    <t>1.098566371</t>
+  </si>
+  <si>
+    <t>0.01295653428</t>
+  </si>
+  <si>
+    <t>1622609.485</t>
+  </si>
+  <si>
+    <t>1731206.074</t>
+  </si>
+  <si>
+    <t>221.8461665</t>
+  </si>
+  <si>
+    <t>237.6345287</t>
+  </si>
+  <si>
+    <t>47486.27077</t>
+  </si>
+  <si>
+    <t>0.1016116051</t>
+  </si>
+  <si>
+    <t>0.01447833686</t>
+  </si>
+  <si>
+    <t>1.487800669</t>
+  </si>
+  <si>
+    <t>0.0097313687</t>
+  </si>
+  <si>
+    <t>575484.9314</t>
+  </si>
+  <si>
+    <t>604178.6231</t>
+  </si>
+  <si>
+    <t>44.99434549</t>
+  </si>
+  <si>
+    <t>48.25156195</t>
+  </si>
+  <si>
+    <t>25031.084</t>
+  </si>
+  <si>
+    <t>0.2713265139</t>
+  </si>
+  <si>
+    <t>0.01640386948</t>
+  </si>
+  <si>
+    <t>0.5680852658</t>
+  </si>
+  <si>
+    <t>0.02887571719</t>
+  </si>
+  <si>
+    <t>1446490.198</t>
+  </si>
+  <si>
+    <t>1671161.101</t>
+  </si>
+  <si>
+    <t>62.76779411</t>
+  </si>
+  <si>
+    <t>67.91596762</t>
   </si>
 </sst>
 </file>
@@ -1174,410 +1235,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80C929F-8CA4-48C8-A979-6F57E314EB1E}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="16.36328125" customWidth="1"/>
-    <col min="11" max="11" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" customWidth="1"/>
+    <col min="8" max="8" width="15.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="16.36328125" customWidth="1"/>
+    <col min="12" max="12" width="15.90625" customWidth="1"/>
+    <col min="13" max="13" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
       <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:13" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="6" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="7" spans="1:13" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="8" spans="1:13" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" t="s">
-        <v>54</v>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="9" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" t="s">
-        <v>62</v>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M9" t="s">
+        <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" t="s">
-        <v>69</v>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K10" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" t="s">
+        <v>111</v>
+      </c>
+      <c r="M10" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="11" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" t="s">
-        <v>91</v>
-      </c>
-      <c r="K10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" t="s">
-        <v>100</v>
-      </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="H11" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="I11" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="J11" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="K11" t="s">
-        <v>97</v>
+        <v>118</v>
+      </c>
+      <c r="L11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>